<commit_message>
docs: Document models and fix Excel export errors
This commit focuses on improving code documentation and correcting existing issues:

- Added module-level docstring to `sys_tdm/sys_tdm/produtos/models.py` for better code clarity and maintainability.
- Corrected indentation errors, removed duplicate lines, and fixed a syntax error in `sys_tdm/sys_tdm/orcamentos/excel_utils.py`.
- Other minor adjustments across `consumos`, `estoque`, `orcamentos`, and `produtos` applications, including:
    - Adding docstrings to forms and admin files.
    - Updating URLs and templates.
    - Refactoring some views for clarity.
</commit_message>
<xml_diff>
--- a/sys_tdm/sys_tdm/static/excel_templates/modelo_impressao_consumo_material.xlsx
+++ b/sys_tdm/sys_tdm/static/excel_templates/modelo_impressao_consumo_material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biasg\OneDrive\Ambiente de Trabalho\Lucas\Projetos\Tudemmad\sys_tdm\sys_tdm\static\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6524D63A-F695-4963-9A7E-10F8821627E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437EA0FE-BF6D-42CB-BCC1-9B72E08DD24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,17 +21,28 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Folha1!$A$1:$F$63</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Cod. Máquina</t>
   </si>
@@ -103,13 +114,16 @@
   </si>
   <si>
     <t>MATÉRIA-PRIMA/COMPONENTES</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +154,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -278,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,12 +320,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,36 +331,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -650,12 +680,13 @@
   </sheetPr>
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F63"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="18"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="4" width="46.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
@@ -742,479 +773,481 @@
       <c r="E7" s="6"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="23" t="s">
+    <row r="8" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="9" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="3"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-    </row>
-    <row r="35" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-    </row>
-    <row r="37" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-    </row>
-    <row r="40" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-    </row>
-    <row r="41" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-    </row>
-    <row r="42" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-    </row>
-    <row r="43" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-    </row>
-    <row r="44" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-    </row>
-    <row r="45" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B45" s="20"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-    </row>
-    <row r="46" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-    </row>
-    <row r="47" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-    </row>
-    <row r="48" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-    </row>
-    <row r="49" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-    </row>
-    <row r="50" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-    </row>
-    <row r="51" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+    <row r="9" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+    </row>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+    </row>
+    <row r="27" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+    </row>
+    <row r="29" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+    </row>
+    <row r="31" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+    </row>
+    <row r="34" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+    </row>
+    <row r="35" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="25"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+    </row>
+    <row r="36" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+    </row>
+    <row r="37" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+    </row>
+    <row r="38" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+    </row>
+    <row r="39" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+    </row>
+    <row r="41" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="25"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+    </row>
+    <row r="43" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="25"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+    </row>
+    <row r="45" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+    </row>
+    <row r="47" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="25"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+    </row>
+    <row r="48" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+    </row>
+    <row r="49" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="25"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+    </row>
+    <row r="50" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+    </row>
+    <row r="51" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="25"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
     </row>
     <row r="52" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
     <row r="53" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="24" t="s">
+      <c r="A53" s="31"/>
+      <c r="B53" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
     </row>
     <row r="54" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B54" s="12"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="14"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="12"/>
     </row>
     <row r="55" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B55" s="15"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="13"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="16"/>
+      <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B56" s="15"/>
+      <c r="B56" s="13"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="16"/>
+      <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B57" s="15"/>
+      <c r="B57" s="13"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
-      <c r="F57" s="16"/>
+      <c r="F57" s="14"/>
     </row>
     <row r="58" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B58" s="15"/>
+      <c r="B58" s="13"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
-      <c r="F58" s="16"/>
+      <c r="F58" s="14"/>
     </row>
     <row r="59" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B59" s="15"/>
+      <c r="B59" s="13"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
-      <c r="F59" s="16"/>
+      <c r="F59" s="14"/>
     </row>
     <row r="60" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B60" s="15"/>
+      <c r="B60" s="13"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="16"/>
+      <c r="F60" s="14"/>
     </row>
     <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B61" s="15"/>
+      <c r="B61" s="13"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
-      <c r="F61" s="16"/>
+      <c r="F61" s="14"/>
     </row>
     <row r="62" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B62" s="15"/>
+      <c r="B62" s="13"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
-      <c r="F62" s="16"/>
+      <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="19"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="48">
@@ -1232,22 +1265,25 @@
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B31:D31"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B36:C36"/>
@@ -1259,13 +1295,10 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B33:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>